<commit_message>
Updated acceptations tests document
</commit_message>
<xml_diff>
--- a/Documents/Tests d'acceptation - Sprint 1.xlsx
+++ b/Documents/Tests d'acceptation - Sprint 1.xlsx
@@ -24,12 +24,6 @@
     <t>Story</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
 Accès à la base de données
 _*Then*_ 
 Les tables, les champs, les types et relations respectent le MCD/MLD</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>État</t>
   </si>
 </sst>
 </file>
@@ -239,17 +239,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -260,6 +290,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:D14" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Colonne1" headerRowDxfId="2" dataDxfId="0"/>
+    <tableColumn id="2" name="Colonne2" headerRowDxfId="3" dataDxfId="1"/>
+    <tableColumn id="3" name="Colonne3" headerRowDxfId="4" dataDxfId="7"/>
+    <tableColumn id="4" name="Colonne4" headerRowDxfId="5" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,221 +570,223 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="78.85546875" style="1" customWidth="1"/>
     <col min="5" max="256" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:D14">
+  <sortState ref="A2:D15">
     <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>